<commit_message>
Working cosine clustering , still not connecting to filter page
</commit_message>
<xml_diff>
--- a/backend/uploads/cosine_clustered_importer_name.xlsx
+++ b/backend/uploads/cosine_clustered_importer_name.xlsx
@@ -1110,7 +1110,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>green (raw) petroleum coke (in bulk)</t>
+          <t>green(raw) petroleum coke (in bulk)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>green (raw) petroleum coke (in bulk)</t>
+          <t>green(raw) petroleum coke (in bulk)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>green (raw) petroleum coke (in bulk)</t>
+          <t>green(raw) petroleum coke (in bulk)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1515,13 +1515,13 @@
         <v>2021</v>
       </c>
       <c r="T12" t="n">
-        <v>2.199</v>
+        <v>2.2023</v>
       </c>
       <c r="U12" t="n">
-        <v>2858.6746</v>
+        <v>2862.9648</v>
       </c>
       <c r="V12" t="n">
-        <v>3.4794</v>
+        <v>3.4846</v>
       </c>
     </row>
     <row r="13">
@@ -1782,10 +1782,10 @@
         <v>2021</v>
       </c>
       <c r="T15" t="n">
-        <v>6.3816</v>
+        <v>6.3818</v>
       </c>
       <c r="U15" t="n">
-        <v>6381394.4829</v>
+        <v>6381553.8694</v>
       </c>
       <c r="V15" t="n">
         <v>0.3487</v>
@@ -1871,10 +1871,10 @@
         <v>2021</v>
       </c>
       <c r="T16" t="n">
-        <v>6.3816</v>
+        <v>6.3818</v>
       </c>
       <c r="U16" t="n">
-        <v>12762788.6936</v>
+        <v>12763107.4665</v>
       </c>
       <c r="V16" t="n">
         <v>0.3487</v>
@@ -1960,10 +1960,10 @@
         <v>2021</v>
       </c>
       <c r="T17" t="n">
-        <v>6.3816</v>
+        <v>6.3818</v>
       </c>
       <c r="U17" t="n">
-        <v>15953485.5266</v>
+        <v>15953883.9929</v>
       </c>
       <c r="V17" t="n">
         <v>0.3487</v>
@@ -2049,10 +2049,10 @@
         <v>2021</v>
       </c>
       <c r="T18" t="n">
-        <v>6.3816</v>
+        <v>6.3818</v>
       </c>
       <c r="U18" t="n">
-        <v>1749427.3163</v>
+        <v>1749471.0113</v>
       </c>
       <c r="V18" t="n">
         <v>0.3487</v>
@@ -2138,10 +2138,10 @@
         <v>2021</v>
       </c>
       <c r="T19" t="n">
-        <v>6.3816</v>
+        <v>6.3818</v>
       </c>
       <c r="U19" t="n">
-        <v>3190697.1053</v>
+        <v>3190776.7986</v>
       </c>
       <c r="V19" t="n">
         <v>0.3487</v>
@@ -3206,13 +3206,13 @@
         <v>2021</v>
       </c>
       <c r="T31" t="n">
-        <v>2.1804</v>
+        <v>2.1837</v>
       </c>
       <c r="U31" t="n">
-        <v>3488.6664</v>
+        <v>3493.902</v>
       </c>
       <c r="V31" t="n">
-        <v>3.4794</v>
+        <v>3.4846</v>
       </c>
     </row>
     <row r="32">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>danblock brakes india private limited</t>
+          <t>brakes india private limited</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
@@ -3473,13 +3473,13 @@
         <v>2021</v>
       </c>
       <c r="T34" t="n">
-        <v>84.8603</v>
+        <v>84.9866</v>
       </c>
       <c r="U34" t="n">
-        <v>848578.9415</v>
+        <v>849841.9051</v>
       </c>
       <c r="V34" t="n">
-        <v>0.8063</v>
+        <v>0.8075</v>
       </c>
     </row>
     <row r="35">
@@ -3562,13 +3562,13 @@
         <v>2021</v>
       </c>
       <c r="T35" t="n">
-        <v>82.96559999999999</v>
+        <v>83.0891</v>
       </c>
       <c r="U35" t="n">
-        <v>331862.4859</v>
+        <v>332356.4061</v>
       </c>
       <c r="V35" t="n">
-        <v>0.8063</v>
+        <v>0.8075</v>
       </c>
     </row>
     <row r="36">
@@ -3651,13 +3651,13 @@
         <v>2021</v>
       </c>
       <c r="T36" t="n">
-        <v>82.96559999999999</v>
+        <v>83.0891</v>
       </c>
       <c r="U36" t="n">
-        <v>331862.4859</v>
+        <v>332356.4061</v>
       </c>
       <c r="V36" t="n">
-        <v>0.8063</v>
+        <v>0.8075</v>
       </c>
     </row>
     <row r="37">
@@ -3740,13 +3740,13 @@
         <v>2021</v>
       </c>
       <c r="T37" t="n">
-        <v>669.501</v>
+        <v>671.8729</v>
       </c>
       <c r="U37" t="n">
-        <v>133899.1807</v>
+        <v>134373.5613</v>
       </c>
       <c r="V37" t="n">
-        <v>8.1991</v>
+        <v>8.228199999999999</v>
       </c>
     </row>
     <row r="38">
@@ -3829,13 +3829,13 @@
         <v>2021</v>
       </c>
       <c r="T38" t="n">
-        <v>79794.2026</v>
+        <v>79928.6032</v>
       </c>
       <c r="U38" t="n">
-        <v>1915060.8625</v>
+        <v>1918286.4776</v>
       </c>
       <c r="V38" t="n">
-        <v>983.2927</v>
+        <v>984.9489</v>
       </c>
     </row>
     <row r="39">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>calcined petroleum coke in bulk</t>
+          <t>calcined petroleum coke</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -4274,13 +4274,13 @@
         <v>2021</v>
       </c>
       <c r="T43" t="n">
-        <v>261910.1694</v>
+        <v>262351.3154</v>
       </c>
       <c r="U43" t="n">
-        <v>1309550.8237</v>
+        <v>1311756.5536</v>
       </c>
       <c r="V43" t="n">
-        <v>2653.1448</v>
+        <v>2657.6136</v>
       </c>
     </row>
     <row r="44">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>graphitized petroleum coke --petroleum coke</t>
+          <t>petroleum coke (graphitized)</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>calcined petroleum coke in bulk</t>
+          <t>calcined petroleum coke</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">

</xml_diff>

<commit_message>
sent a copy to Nidhi
</commit_message>
<xml_diff>
--- a/backend/uploads/cosine_clustered_importer_name.xlsx
+++ b/backend/uploads/cosine_clustered_importer_name.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1515,13 +1522,13 @@
         <v>2021</v>
       </c>
       <c r="T12" t="n">
-        <v>2.2023</v>
+        <v>2.2005</v>
       </c>
       <c r="U12" t="n">
-        <v>2862.9648</v>
+        <v>2860.6286</v>
       </c>
       <c r="V12" t="n">
-        <v>3.4846</v>
+        <v>3.4818</v>
       </c>
     </row>
     <row r="13">
@@ -1614,91 +1621,92 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>import</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>2018-04-01</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>krishnapatnam port sea (inkri1)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>2018-04-07 00:00:00</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="2" t="n">
         <v>27131100</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>saudi arabia</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr"/>
+      <c r="H14" s="2" t="inlineStr">
         <is>
           <t>petroleum coke</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="2" t="inlineStr">
         <is>
           <t>usd</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="2" t="n">
         <v>106.44</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="2" t="n">
         <v>25000000</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" s="2" t="inlineStr">
         <is>
           <t>kgs</t>
         </is>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" s="2" t="n">
         <v>6939.4</v>
       </c>
-      <c r="N14" t="n">
+      <c r="N14" s="2" t="n">
         <v>173485036.82</v>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="O14" s="2" t="inlineStr">
         <is>
           <t>sinopec international middle east</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>ultratech cement limited</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <t>zuari cement limited</t>
+        </is>
+      </c>
+      <c r="Q14" s="2" t="inlineStr">
         <is>
           <t>andheri e mumbai maharashtra</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="R14" s="2" t="inlineStr">
         <is>
           <t>january</t>
         </is>
       </c>
-      <c r="S14" t="n">
+      <c r="S14" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="T14" t="n">
+      <c r="T14" s="2" t="n">
         <v>6939.4</v>
       </c>
-      <c r="U14" t="n">
+      <c r="U14" s="2" t="n">
         <v>173485036.82</v>
       </c>
-      <c r="V14" t="n">
+      <c r="V14" s="2" t="n">
         <v>106.44</v>
       </c>
     </row>
@@ -1782,10 +1790,10 @@
         <v>2021</v>
       </c>
       <c r="T15" t="n">
-        <v>6.3818</v>
+        <v>6.3817</v>
       </c>
       <c r="U15" t="n">
-        <v>6381553.8694</v>
+        <v>6381471.8322</v>
       </c>
       <c r="V15" t="n">
         <v>0.3487</v>
@@ -1871,10 +1879,10 @@
         <v>2021</v>
       </c>
       <c r="T16" t="n">
-        <v>6.3818</v>
+        <v>6.3817</v>
       </c>
       <c r="U16" t="n">
-        <v>12763107.4665</v>
+        <v>12762943.3922</v>
       </c>
       <c r="V16" t="n">
         <v>0.3487</v>
@@ -1960,10 +1968,10 @@
         <v>2021</v>
       </c>
       <c r="T17" t="n">
-        <v>6.3818</v>
+        <v>6.3817</v>
       </c>
       <c r="U17" t="n">
-        <v>15953883.9929</v>
+        <v>15953678.8999</v>
       </c>
       <c r="V17" t="n">
         <v>0.3487</v>
@@ -2049,10 +2057,10 @@
         <v>2021</v>
       </c>
       <c r="T18" t="n">
-        <v>6.3818</v>
+        <v>6.3817</v>
       </c>
       <c r="U18" t="n">
-        <v>1749471.0113</v>
+        <v>1749448.5212</v>
       </c>
       <c r="V18" t="n">
         <v>0.3487</v>
@@ -2138,10 +2146,10 @@
         <v>2021</v>
       </c>
       <c r="T19" t="n">
-        <v>6.3818</v>
+        <v>6.3817</v>
       </c>
       <c r="U19" t="n">
-        <v>3190776.7986</v>
+        <v>3190735.78</v>
       </c>
       <c r="V19" t="n">
         <v>0.3487</v>
@@ -3206,101 +3214,102 @@
         <v>2021</v>
       </c>
       <c r="T31" t="n">
-        <v>2.1837</v>
+        <v>2.1819</v>
       </c>
       <c r="U31" t="n">
-        <v>3493.902</v>
+        <v>3491.0509</v>
       </c>
       <c r="V31" t="n">
-        <v>3.4846</v>
+        <v>3.4818</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>import</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>2018-05-01</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>chennai sea (inmaa1)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="2" t="inlineStr">
         <is>
           <t>2018-05-08 00:00:00</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" s="2" t="n">
         <v>27131200</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" s="2" t="inlineStr">
         <is>
           <t>china</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="G32" s="2" t="inlineStr"/>
+      <c r="H32" s="2" t="inlineStr">
         <is>
           <t>carburiser graph-hex 98 (1-5mm sizing)</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" s="2" t="inlineStr">
         <is>
           <t>usd</t>
         </is>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="2" t="n">
         <v>0.83</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K32" s="2" t="n">
         <v>21000</v>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="L32" s="2" t="inlineStr">
         <is>
           <t>kgs</t>
         </is>
       </c>
-      <c r="M32" t="n">
+      <c r="M32" s="2" t="n">
         <v>56.02</v>
       </c>
-      <c r="N32" t="n">
+      <c r="N32" s="2" t="n">
         <v>1176525</v>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="O32" s="2" t="inlineStr">
         <is>
           <t>larpen metallurgical service</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>brakes india private limited</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
+      <c r="P32" s="2" t="inlineStr">
+        <is>
+          <t>continental india private limited</t>
+        </is>
+      </c>
+      <c r="Q32" s="2" t="inlineStr">
         <is>
           <t>chennai tamil nadu</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="R32" s="2" t="inlineStr">
         <is>
           <t>january</t>
         </is>
       </c>
-      <c r="S32" t="n">
+      <c r="S32" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="T32" t="n">
+      <c r="T32" s="2" t="n">
         <v>56.02</v>
       </c>
-      <c r="U32" t="n">
+      <c r="U32" s="2" t="n">
         <v>1176525</v>
       </c>
-      <c r="V32" t="n">
+      <c r="V32" s="2" t="n">
         <v>0.83</v>
       </c>
     </row>
@@ -3394,92 +3403,93 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>import</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>2018-05-01</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="2" t="inlineStr">
         <is>
           <t>sonepat icd</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="2" t="inlineStr">
         <is>
           <t>2018-05-10 00:00:00</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" s="2" t="n">
         <v>27131200</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" s="2" t="inlineStr">
         <is>
           <t>united kingdom</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="G34" s="2" t="inlineStr"/>
+      <c r="H34" s="2" t="inlineStr">
         <is>
           <t>d44 petroleum coke (01x0397) (for manufof disc brake pads)( for captive consumption)</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" s="2" t="inlineStr">
         <is>
           <t>gbp</t>
         </is>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="L34" t="inlineStr">
+      <c r="L34" s="2" t="inlineStr">
         <is>
           <t>kgs</t>
         </is>
       </c>
-      <c r="M34" t="n">
+      <c r="M34" s="2" t="n">
         <v>63.15</v>
       </c>
-      <c r="N34" t="n">
+      <c r="N34" s="2" t="n">
         <v>631481.8100000001</v>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="O34" s="2" t="inlineStr">
         <is>
           <t>ms james durrans sons</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
+      <c r="P34" s="2" t="inlineStr">
         <is>
           <t>brakes india private limited</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr">
+      <c r="Q34" s="2" t="inlineStr">
         <is>
           <t>delhi</t>
         </is>
       </c>
-      <c r="R34" t="inlineStr">
+      <c r="R34" s="2" t="inlineStr">
         <is>
           <t>january</t>
         </is>
       </c>
-      <c r="S34" t="n">
+      <c r="S34" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="T34" t="n">
-        <v>84.9866</v>
-      </c>
-      <c r="U34" t="n">
-        <v>849841.9051</v>
-      </c>
-      <c r="V34" t="n">
-        <v>0.8075</v>
+      <c r="T34" s="2" t="n">
+        <v>84.8843</v>
+      </c>
+      <c r="U34" s="2" t="n">
+        <v>848818.9044999999</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0.8065</v>
       </c>
     </row>
     <row r="35">
@@ -3562,13 +3572,13 @@
         <v>2021</v>
       </c>
       <c r="T35" t="n">
-        <v>83.0891</v>
+        <v>82.98909999999999</v>
       </c>
       <c r="U35" t="n">
-        <v>332356.4061</v>
+        <v>331956.3307</v>
       </c>
       <c r="V35" t="n">
-        <v>0.8075</v>
+        <v>0.8065</v>
       </c>
     </row>
     <row r="36">
@@ -3651,13 +3661,13 @@
         <v>2021</v>
       </c>
       <c r="T36" t="n">
-        <v>83.0891</v>
+        <v>82.98909999999999</v>
       </c>
       <c r="U36" t="n">
-        <v>332356.4061</v>
+        <v>331956.3307</v>
       </c>
       <c r="V36" t="n">
-        <v>0.8075</v>
+        <v>0.8065</v>
       </c>
     </row>
     <row r="37">
@@ -3740,13 +3750,13 @@
         <v>2021</v>
       </c>
       <c r="T37" t="n">
-        <v>671.8729</v>
+        <v>671.5915</v>
       </c>
       <c r="U37" t="n">
-        <v>134373.5613</v>
+        <v>134317.2859</v>
       </c>
       <c r="V37" t="n">
-        <v>8.228199999999999</v>
+        <v>8.2247</v>
       </c>
     </row>
     <row r="38">
@@ -3829,13 +3839,13 @@
         <v>2021</v>
       </c>
       <c r="T38" t="n">
-        <v>79928.6032</v>
+        <v>79873.7458</v>
       </c>
       <c r="U38" t="n">
-        <v>1918286.4776</v>
+        <v>1916969.9</v>
       </c>
       <c r="V38" t="n">
-        <v>984.9489</v>
+        <v>984.2729</v>
       </c>
     </row>
     <row r="39">
@@ -4274,13 +4284,13 @@
         <v>2021</v>
       </c>
       <c r="T43" t="n">
-        <v>262351.3154</v>
+        <v>262171.2558</v>
       </c>
       <c r="U43" t="n">
-        <v>1311756.5536</v>
+        <v>1310856.2557</v>
       </c>
       <c r="V43" t="n">
-        <v>2657.6136</v>
+        <v>2655.7896</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
going to send to nidhi
</commit_message>
<xml_diff>
--- a/backend/uploads/cosine_clustered_importer_name.xlsx
+++ b/backend/uploads/cosine_clustered_importer_name.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1521,15 +1521,6 @@
       <c r="S12" t="n">
         <v>2021</v>
       </c>
-      <c r="T12" t="n">
-        <v>2.2005</v>
-      </c>
-      <c r="U12" t="n">
-        <v>2860.6286</v>
-      </c>
-      <c r="V12" t="n">
-        <v>3.4818</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1621,92 +1612,91 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>import</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>2018-04-01</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>krishnapatnam port sea (inkri1)</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>2018-04-07 00:00:00</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" t="n">
         <v>27131100</v>
       </c>
-      <c r="F14" s="2" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>saudi arabia</t>
         </is>
       </c>
-      <c r="G14" s="2" t="inlineStr"/>
-      <c r="H14" s="2" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>petroleum coke</t>
         </is>
       </c>
-      <c r="I14" s="2" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>usd</t>
         </is>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" t="n">
         <v>106.44</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" t="n">
         <v>25000000</v>
       </c>
-      <c r="L14" s="2" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>kgs</t>
         </is>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="M14" t="n">
         <v>6939.4</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="N14" t="n">
         <v>173485036.82</v>
       </c>
-      <c r="O14" s="2" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>sinopec international middle east</t>
         </is>
       </c>
-      <c r="P14" s="2" t="inlineStr">
-        <is>
-          <t>zuari cement limited</t>
-        </is>
-      </c>
-      <c r="Q14" s="2" t="inlineStr">
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>ultratech cement limited</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>andheri e mumbai maharashtra</t>
         </is>
       </c>
-      <c r="R14" s="2" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>january</t>
         </is>
       </c>
-      <c r="S14" s="2" t="n">
+      <c r="S14" t="n">
         <v>2021</v>
       </c>
-      <c r="T14" s="2" t="n">
+      <c r="T14" t="n">
         <v>6939.4</v>
       </c>
-      <c r="U14" s="2" t="n">
+      <c r="U14" t="n">
         <v>173485036.82</v>
       </c>
-      <c r="V14" s="2" t="n">
+      <c r="V14" t="n">
         <v>106.44</v>
       </c>
     </row>
@@ -1789,15 +1779,6 @@
       <c r="S15" t="n">
         <v>2021</v>
       </c>
-      <c r="T15" t="n">
-        <v>6.3817</v>
-      </c>
-      <c r="U15" t="n">
-        <v>6381471.8322</v>
-      </c>
-      <c r="V15" t="n">
-        <v>0.3487</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1878,15 +1859,6 @@
       <c r="S16" t="n">
         <v>2021</v>
       </c>
-      <c r="T16" t="n">
-        <v>6.3817</v>
-      </c>
-      <c r="U16" t="n">
-        <v>12762943.3922</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0.3487</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1967,15 +1939,6 @@
       <c r="S17" t="n">
         <v>2021</v>
       </c>
-      <c r="T17" t="n">
-        <v>6.3817</v>
-      </c>
-      <c r="U17" t="n">
-        <v>15953678.8999</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.3487</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2056,15 +2019,6 @@
       <c r="S18" t="n">
         <v>2021</v>
       </c>
-      <c r="T18" t="n">
-        <v>6.3817</v>
-      </c>
-      <c r="U18" t="n">
-        <v>1749448.5212</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0.3487</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2145,15 +2099,6 @@
       <c r="S19" t="n">
         <v>2021</v>
       </c>
-      <c r="T19" t="n">
-        <v>6.3817</v>
-      </c>
-      <c r="U19" t="n">
-        <v>3190735.78</v>
-      </c>
-      <c r="V19" t="n">
-        <v>0.3487</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3213,103 +3158,93 @@
       <c r="S31" t="n">
         <v>2021</v>
       </c>
-      <c r="T31" t="n">
-        <v>2.1819</v>
-      </c>
-      <c r="U31" t="n">
-        <v>3491.0509</v>
-      </c>
-      <c r="V31" t="n">
-        <v>3.4818</v>
-      </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>import</t>
         </is>
       </c>
-      <c r="B32" s="2" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>2018-05-01</t>
         </is>
       </c>
-      <c r="C32" s="2" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>chennai sea (inmaa1)</t>
         </is>
       </c>
-      <c r="D32" s="2" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>2018-05-08 00:00:00</t>
         </is>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" t="n">
         <v>27131200</v>
       </c>
-      <c r="F32" s="2" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>china</t>
         </is>
       </c>
-      <c r="G32" s="2" t="inlineStr"/>
-      <c r="H32" s="2" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>carburiser graph-hex 98 (1-5mm sizing)</t>
         </is>
       </c>
-      <c r="I32" s="2" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>usd</t>
         </is>
       </c>
-      <c r="J32" s="2" t="n">
+      <c r="J32" t="n">
         <v>0.83</v>
       </c>
-      <c r="K32" s="2" t="n">
+      <c r="K32" t="n">
         <v>21000</v>
       </c>
-      <c r="L32" s="2" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>kgs</t>
         </is>
       </c>
-      <c r="M32" s="2" t="n">
+      <c r="M32" t="n">
         <v>56.02</v>
       </c>
-      <c r="N32" s="2" t="n">
+      <c r="N32" t="n">
         <v>1176525</v>
       </c>
-      <c r="O32" s="2" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t>larpen metallurgical service</t>
         </is>
       </c>
-      <c r="P32" s="2" t="inlineStr">
-        <is>
-          <t>continental india private limited</t>
-        </is>
-      </c>
-      <c r="Q32" s="2" t="inlineStr">
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>brakes india private limited</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>chennai tamil nadu</t>
         </is>
       </c>
-      <c r="R32" s="2" t="inlineStr">
+      <c r="R32" t="inlineStr">
         <is>
           <t>january</t>
         </is>
       </c>
-      <c r="S32" s="2" t="n">
+      <c r="S32" t="n">
         <v>2021</v>
       </c>
-      <c r="T32" s="2" t="n">
+      <c r="T32" t="n">
         <v>56.02</v>
       </c>
-      <c r="U32" s="2" t="n">
+      <c r="U32" t="n">
         <v>1176525</v>
       </c>
-      <c r="V32" s="2" t="n">
+      <c r="V32" t="n">
         <v>0.83</v>
       </c>
     </row>
@@ -3482,15 +3417,9 @@
       <c r="S34" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="T34" s="2" t="n">
-        <v>84.8843</v>
-      </c>
-      <c r="U34" s="2" t="n">
-        <v>848818.9044999999</v>
-      </c>
-      <c r="V34" s="2" t="n">
-        <v>0.8065</v>
-      </c>
+      <c r="T34" s="2" t="inlineStr"/>
+      <c r="U34" s="2" t="inlineStr"/>
+      <c r="V34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3571,15 +3500,6 @@
       <c r="S35" t="n">
         <v>2021</v>
       </c>
-      <c r="T35" t="n">
-        <v>82.98909999999999</v>
-      </c>
-      <c r="U35" t="n">
-        <v>331956.3307</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0.8065</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3660,15 +3580,6 @@
       <c r="S36" t="n">
         <v>2021</v>
       </c>
-      <c r="T36" t="n">
-        <v>82.98909999999999</v>
-      </c>
-      <c r="U36" t="n">
-        <v>331956.3307</v>
-      </c>
-      <c r="V36" t="n">
-        <v>0.8065</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3749,15 +3660,6 @@
       <c r="S37" t="n">
         <v>2021</v>
       </c>
-      <c r="T37" t="n">
-        <v>671.5915</v>
-      </c>
-      <c r="U37" t="n">
-        <v>134317.2859</v>
-      </c>
-      <c r="V37" t="n">
-        <v>8.2247</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3838,15 +3740,6 @@
       <c r="S38" t="n">
         <v>2021</v>
       </c>
-      <c r="T38" t="n">
-        <v>79873.7458</v>
-      </c>
-      <c r="U38" t="n">
-        <v>1916969.9</v>
-      </c>
-      <c r="V38" t="n">
-        <v>984.2729</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4283,15 +4176,6 @@
       <c r="S43" t="n">
         <v>2021</v>
       </c>
-      <c r="T43" t="n">
-        <v>262171.2558</v>
-      </c>
-      <c r="U43" t="n">
-        <v>1310856.2557</v>
-      </c>
-      <c r="V43" t="n">
-        <v>2655.7896</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4514,7 +4398,7 @@
         <v>485</v>
       </c>
       <c r="K46" t="n">
-        <v>5198000</v>
+        <v>50000</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -4557,6 +4441,362 @@
         <v>173074128.2</v>
       </c>
       <c r="V46" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>import</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2019-08-01</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>kakinada sea (inkak1)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2018-05-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>27131200</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>united states</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>calcined petroleum coke</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>usd</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
+        <v>485</v>
+      </c>
+      <c r="K47" t="n">
+        <v>100000</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>kgs</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="N47" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>oxbow calcining international</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>vedanta limited</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>panajigoa</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>january</t>
+        </is>
+      </c>
+      <c r="S47" t="n">
+        <v>2021</v>
+      </c>
+      <c r="T47" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="U47" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="V47" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>import</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2020-06-01</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>kakinada sea (inkak1)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2018-05-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>27131200</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>united states</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>calcined petroleum coke in bulk</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>usd</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
+        <v>485</v>
+      </c>
+      <c r="K48" t="n">
+        <v>150000</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>kgs</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="N48" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>oxbow calcining international</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>vedanta limited</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>panajigoa</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>january</t>
+        </is>
+      </c>
+      <c r="S48" t="n">
+        <v>2021</v>
+      </c>
+      <c r="T48" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="U48" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="V48" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>import</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2021-07-01</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>kakinada sea (inkak1)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2018-05-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>27131200</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>united states</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>calcined petroleum coke in bulk</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>usd</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
+        <v>485</v>
+      </c>
+      <c r="K49" t="n">
+        <v>180000</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>kgs</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="N49" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>oxbow calcining international</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>vedanta limited</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>panajigoa</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>january</t>
+        </is>
+      </c>
+      <c r="S49" t="n">
+        <v>2021</v>
+      </c>
+      <c r="T49" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="U49" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="V49" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>import</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2022-12-01</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>kakinada sea (inkak1)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2018-05-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>27131200</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>united states</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>calcined petroleum coke in bulk</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>usd</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
+        <v>485</v>
+      </c>
+      <c r="K50" t="n">
+        <v>190000</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>kgs</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="N50" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>oxbow calcining international</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>vedanta limited</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>panajigoa</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>january</t>
+        </is>
+      </c>
+      <c r="S50" t="n">
+        <v>2021</v>
+      </c>
+      <c r="T50" t="n">
+        <v>33296.29</v>
+      </c>
+      <c r="U50" t="n">
+        <v>173074128.2</v>
+      </c>
+      <c r="V50" t="n">
         <v>485</v>
       </c>
     </row>

</xml_diff>

<commit_message>
before making analysis catalog pretty
</commit_message>
<xml_diff>
--- a/backend/uploads/cosine_clustered_importer_name.xlsx
+++ b/backend/uploads/cosine_clustered_importer_name.xlsx
@@ -29,18 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -61,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1295,7 +1288,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>green(raw) petroleum coke (in bulk)</t>
+          <t>green (raw) petroleum coke (in bulk)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1384,7 +1377,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>green(raw) petroleum coke (in bulk)</t>
+          <t>green (raw) petroleum coke (in bulk)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -3338,88 +3331,84 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>import</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>import</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>2018-05-01</t>
         </is>
       </c>
-      <c r="C34" s="2" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>sonepat icd</t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>2018-05-10 00:00:00</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" t="n">
         <v>27131200</v>
       </c>
-      <c r="F34" s="2" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>united kingdom</t>
         </is>
       </c>
-      <c r="G34" s="2" t="inlineStr"/>
-      <c r="H34" s="2" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>d44 petroleum coke (01x0397) (for manufof disc brake pads)( for captive consumption)</t>
         </is>
       </c>
-      <c r="I34" s="2" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>gbp</t>
         </is>
       </c>
-      <c r="J34" s="2" t="n">
+      <c r="J34" t="n">
         <v>0.6</v>
       </c>
-      <c r="K34" s="2" t="n">
+      <c r="K34" t="n">
         <v>10000</v>
       </c>
-      <c r="L34" s="2" t="inlineStr">
-        <is>
-          <t>kgs</t>
-        </is>
-      </c>
-      <c r="M34" s="2" t="n">
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>kgs</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
         <v>63.15</v>
       </c>
-      <c r="N34" s="2" t="n">
+      <c r="N34" t="n">
         <v>631481.8100000001</v>
       </c>
-      <c r="O34" s="2" t="inlineStr">
+      <c r="O34" t="inlineStr">
         <is>
           <t>ms james durrans sons</t>
         </is>
       </c>
-      <c r="P34" s="2" t="inlineStr">
-        <is>
-          <t>brakes india private limited</t>
-        </is>
-      </c>
-      <c r="Q34" s="2" t="inlineStr">
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>danblock brakes india private limited</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>delhi</t>
         </is>
       </c>
-      <c r="R34" s="2" t="inlineStr">
-        <is>
-          <t>january</t>
-        </is>
-      </c>
-      <c r="S34" s="2" t="n">
-        <v>2021</v>
-      </c>
-      <c r="T34" s="2" t="inlineStr"/>
-      <c r="U34" s="2" t="inlineStr"/>
-      <c r="V34" s="2" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>january</t>
+        </is>
+      </c>
+      <c r="S34" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4386,7 +4375,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>calcined petroleum coke</t>
+          <t>calcined petroleum coke in bulk</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -4475,7 +4464,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>calcined petroleum coke</t>
+          <t>calcined petroleum coke in bulk</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">

</xml_diff>